<commit_message>
BF:typos and wrong places for some translations.
</commit_message>
<xml_diff>
--- a/docs/i18n_unique_strings.xlsx
+++ b/docs/i18n_unique_strings.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="360">
   <si>
     <t>You are not the line manager of this employee. You cannot reject this overtime request.</t>
   </si>
@@ -1027,6 +1027,75 @@
   </si>
   <si>
     <t>please respect the format</t>
+  </si>
+  <si>
+    <t>The overtime you've requested has been rejected. Below, the details :</t>
+  </si>
+  <si>
+    <t>The overtime you've requested has been accepted. Below, the details :</t>
+  </si>
+  <si>
+    <t>{Firstname} {Lastname} requests an overtime. Below, the details :</t>
+  </si>
+  <si>
+    <t>Once connected, you can change your password, as explained here.</t>
+  </si>
+  <si>
+    <t>The leave you've requested has been rejected. Below, the details :</t>
+  </si>
+  <si>
+    <t>The leave you've requested has been accepted. Below, the details :</t>
+  </si>
+  <si>
+    <t>{Firstname} {Lastname} requests a leave. Below, the details :</t>
+  </si>
+  <si>
+    <t>From</t>
+  </si>
+  <si>
+    <t>To</t>
+  </si>
+  <si>
+    <t>Dear {Firstname} {Lastname},</t>
+  </si>
+  <si>
+    <t>If you didn't perform this operation, please contact your administrator.</t>
+  </si>
+  <si>
+    <t>Welcome in LMS. If your are an employee, you could now :</t>
+  </si>
+  <si>
+    <t>See your leave balance.</t>
+  </si>
+  <si>
+    <t>See the list of the leave requests you have submitted.</t>
+  </si>
+  <si>
+    <t>Request a new leave.</t>
+  </si>
+  <si>
+    <t>If your are the line manager of other employee(s), you could now :</t>
+  </si>
+  <si>
+    <t>Validate leave requests submitted to you.</t>
+  </si>
+  <si>
+    <t>Validate overtime requests submitted to you.</t>
+  </si>
+  <si>
+    <t>Access forbidden</t>
+  </si>
+  <si>
+    <t>You are not allowed to perform this action.</t>
+  </si>
+  <si>
+    <t>don't remove or replace {Firstname} and {Lastname}</t>
+  </si>
+  <si>
+    <t>Welcome to LMS {Firstname} {Lastname}. Please use these credentials to login to the system:</t>
+  </si>
+  <si>
+    <t>In the sense of overtime (extra hours)</t>
   </si>
 </sst>
 </file>
@@ -1377,10 +1446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B319"/>
+  <dimension ref="A1:B340"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A303" workbookViewId="0">
-      <selection activeCell="A319" sqref="A2:A319"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A329" sqref="A329"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3057,6 +3126,9 @@
       <c r="A311" t="s">
         <v>303</v>
       </c>
+      <c r="B311" t="s">
+        <v>359</v>
+      </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
@@ -3102,6 +3174,120 @@
     <row r="319" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>308</v>
+      </c>
+    </row>
+    <row r="320" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A320" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="321" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A321" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="322" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A322" t="s">
+        <v>339</v>
+      </c>
+      <c r="B322" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="323" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A323" t="s">
+        <v>358</v>
+      </c>
+      <c r="B323" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="324" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A324" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="325" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A325" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="326" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A326" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="327" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A327" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="328" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A328" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="329" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A329" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="330" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A330" t="s">
+        <v>346</v>
+      </c>
+      <c r="B330" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="331" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A331" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="332" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A332" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="333" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A333" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="334" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A334" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="335" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A335" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="336" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A336" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="337" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A337" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="338" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A338" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="339" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A339" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="340" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A340" t="s">
+        <v>356</v>
       </c>
     </row>
   </sheetData>

</xml_diff>